<commit_message>
Implment data from api to my-requests #2
</commit_message>
<xml_diff>
--- a/Sprints.xlsx
+++ b/Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEST\Linkdev\New-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED09857-926E-47D8-BAD7-CAF9F31A0DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104BEE81-E913-4C92-92F2-427F16B78B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>My Requests</t>
   </si>
   <si>
-    <t>Event details</t>
-  </si>
-  <si>
     <t>setup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events Landing </t>
   </si>
   <si>
     <t>Workspace Dashboard</t>
@@ -165,6 +159,64 @@
   </si>
   <si>
     <t>Date Range (From -to)</t>
+  </si>
+  <si>
+    <t>Est. Time</t>
+  </si>
+  <si>
+    <t>4 Hours</t>
+  </si>
+  <si>
+    <t>Events Landing  &amp; Event details</t>
+  </si>
+  <si>
+    <t>As a user, I want to click on an "Events" link to see a list of upcoming events. (Events Landing)</t>
+  </si>
+  <si>
+    <t>As a user, I want the Events Landing page to display event details like name, date, image, category, description, and location. (Events Landing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a user, I want to see a maximum of 6 upcoming events with paging enabled for older events. (Events Landing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a user, I want to filter events by date, category, or available tickets. (Events Landing)</t>
+  </si>
+  <si>
+    <t>As a user, I want events to be sorted by date in ascending order. (Events Landing)</t>
+  </si>
+  <si>
+    <t>As a user, I want to click on an event name to see its detailed information on a separate page. (Event Details)</t>
+  </si>
+  <si>
+    <t>As a user, I want the Event Details page to display additional information like end date and event tickets. (Event Details)</t>
+  </si>
+  <si>
+    <t>As a user, I want a "Register Now" button to register for an event, redirecting me to the registration page. (Event Details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As a user, I shouldn't be able to register for events that have already passed. (Event Details)</t>
+  </si>
+  <si>
+    <t>US-07</t>
+  </si>
+  <si>
+    <t>US-08</t>
+  </si>
+  <si>
+    <t>US-09</t>
+  </si>
+  <si>
+    <t>Develop API calls to fetch event data from events_category-listing and events_listing endpoints.</t>
+  </si>
+  <si>
+    <t>Design and implement the Events Landing page with filtering and sorting functionalities.</t>
+  </si>
+  <si>
+    <t>Design and implement the Event Details page with registration button.
+Implement logic to check for past events and disable registration.</t>
+  </si>
+  <si>
+    <t>T-03</t>
   </si>
 </sst>
 </file>
@@ -530,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H30"/>
+  <dimension ref="A2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -546,87 +598,91 @@
     <col min="6" max="6" width="58.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="23.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="8"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4" t="s">
+    <row r="9" spans="1:9">
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
+    <row r="10" spans="1:9">
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -634,93 +690,181 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
+    <row r="13" spans="1:9" ht="30">
       <c r="C13" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30">
+      <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="30">
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30">
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:9" ht="45">
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45">
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60">
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30">
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30">
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30">
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30">
+      <c r="C24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30">
+      <c r="C25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30">
+      <c r="C26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2">
+      <c r="B32" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2">
-        <v>3</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>